<commit_message>
Uploading the MIDIScaled Test and Spec doc changes
the MIDIScaled test was an implementation of Littlescale's Midi
framework.  However, I forgot to upload it last week.  Cleon's new work
has made most of it obsolete, which is awesome!  However, I wanted to
post it for the record. :)
</commit_message>
<xml_diff>
--- a/Documents/ASA_YM2612_Custom_Specifications.xlsx
+++ b/Documents/ASA_YM2612_Custom_Specifications.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MIDI Mapping" sheetId="2" r:id="rId1"/>
     <sheet name="YM2612 Memory Maps" sheetId="5" r:id="rId2"/>
-    <sheet name="Tuning" sheetId="1" r:id="rId3"/>
-    <sheet name="MIDI Commands" sheetId="6" r:id="rId4"/>
-    <sheet name="How Things Work" sheetId="3" r:id="rId5"/>
+    <sheet name="How Things Work" sheetId="3" r:id="rId3"/>
+    <sheet name="Tuning" sheetId="1" r:id="rId4"/>
+    <sheet name="MIDI Commands" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tuning!$E$1:$E$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tuning!$E$1:$E$133</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -4426,6 +4426,63 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4433,9 +4490,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4546,60 +4600,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4633,12 +4633,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4659,6 +4653,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5546,7 +5546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC121"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -5564,37 +5564,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="85" customFormat="1" ht="19" thickBot="1">
-      <c r="A1" s="410" t="s">
+      <c r="A1" s="428" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="411"/>
-      <c r="C1" s="411"/>
-      <c r="D1" s="411"/>
-      <c r="E1" s="411"/>
-      <c r="F1" s="411"/>
-      <c r="G1" s="411"/>
-      <c r="H1" s="411"/>
-      <c r="I1" s="411"/>
-      <c r="J1" s="411"/>
-      <c r="K1" s="411"/>
-      <c r="L1" s="411"/>
-      <c r="M1" s="411"/>
-      <c r="N1" s="411"/>
-      <c r="O1" s="411"/>
-      <c r="P1" s="411"/>
-      <c r="Q1" s="411"/>
-      <c r="R1" s="411"/>
-      <c r="S1" s="411"/>
-      <c r="T1" s="411"/>
-      <c r="U1" s="411"/>
-      <c r="V1" s="411"/>
-      <c r="W1" s="411"/>
-      <c r="X1" s="411"/>
-      <c r="Y1" s="411"/>
-      <c r="Z1" s="411"/>
-      <c r="AA1" s="411"/>
-      <c r="AB1" s="411"/>
-      <c r="AC1" s="412"/>
+      <c r="B1" s="429"/>
+      <c r="C1" s="429"/>
+      <c r="D1" s="429"/>
+      <c r="E1" s="429"/>
+      <c r="F1" s="429"/>
+      <c r="G1" s="429"/>
+      <c r="H1" s="429"/>
+      <c r="I1" s="429"/>
+      <c r="J1" s="429"/>
+      <c r="K1" s="429"/>
+      <c r="L1" s="429"/>
+      <c r="M1" s="429"/>
+      <c r="N1" s="429"/>
+      <c r="O1" s="429"/>
+      <c r="P1" s="429"/>
+      <c r="Q1" s="429"/>
+      <c r="R1" s="429"/>
+      <c r="S1" s="429"/>
+      <c r="T1" s="429"/>
+      <c r="U1" s="429"/>
+      <c r="V1" s="429"/>
+      <c r="W1" s="429"/>
+      <c r="X1" s="429"/>
+      <c r="Y1" s="429"/>
+      <c r="Z1" s="429"/>
+      <c r="AA1" s="429"/>
+      <c r="AB1" s="429"/>
+      <c r="AC1" s="430"/>
     </row>
     <row r="2" spans="1:29" s="13" customFormat="1">
       <c r="A2" s="268"/>
@@ -5609,29 +5609,29 @@
       <c r="J2" s="273"/>
       <c r="K2" s="273"/>
       <c r="L2" s="281"/>
-      <c r="M2" s="437" t="s">
+      <c r="M2" s="455" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="438"/>
-      <c r="O2" s="438"/>
-      <c r="P2" s="438"/>
-      <c r="Q2" s="438"/>
+      <c r="N2" s="456"/>
+      <c r="O2" s="456"/>
+      <c r="P2" s="456"/>
+      <c r="Q2" s="456"/>
       <c r="R2" s="288" t="s">
         <v>170</v>
       </c>
-      <c r="S2" s="435" t="s">
+      <c r="S2" s="453" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="436"/>
-      <c r="U2" s="436"/>
+      <c r="T2" s="454"/>
+      <c r="U2" s="454"/>
       <c r="V2" s="289" t="s">
         <v>194</v>
       </c>
-      <c r="W2" s="439" t="s">
+      <c r="W2" s="457" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="440"/>
-      <c r="Y2" s="441"/>
+      <c r="X2" s="458"/>
+      <c r="Y2" s="459"/>
       <c r="Z2" s="290"/>
       <c r="AA2" s="290"/>
       <c r="AB2" s="290"/>
@@ -5918,20 +5918,20 @@
       <c r="AC6" s="297"/>
     </row>
     <row r="7" spans="1:29" s="13" customFormat="1" ht="19" thickBot="1">
-      <c r="A7" s="421" t="s">
+      <c r="A7" s="439" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="422"/>
-      <c r="C7" s="423"/>
-      <c r="D7" s="424"/>
-      <c r="E7" s="425"/>
-      <c r="F7" s="423"/>
-      <c r="G7" s="426"/>
-      <c r="H7" s="426"/>
-      <c r="I7" s="424"/>
-      <c r="J7" s="424"/>
-      <c r="K7" s="425"/>
-      <c r="L7" s="421"/>
+      <c r="B7" s="440"/>
+      <c r="C7" s="441"/>
+      <c r="D7" s="442"/>
+      <c r="E7" s="443"/>
+      <c r="F7" s="441"/>
+      <c r="G7" s="444"/>
+      <c r="H7" s="444"/>
+      <c r="I7" s="442"/>
+      <c r="J7" s="442"/>
+      <c r="K7" s="443"/>
+      <c r="L7" s="439"/>
       <c r="M7" s="294"/>
       <c r="N7" s="56"/>
       <c r="O7" s="56"/>
@@ -5955,19 +5955,19 @@
       <c r="B8" s="191" t="s">
         <v>336</v>
       </c>
-      <c r="C8" s="427" t="s">
+      <c r="C8" s="445" t="s">
         <v>337</v>
       </c>
-      <c r="D8" s="428"/>
-      <c r="E8" s="429"/>
-      <c r="F8" s="427" t="s">
+      <c r="D8" s="446"/>
+      <c r="E8" s="447"/>
+      <c r="F8" s="445" t="s">
         <v>340</v>
       </c>
-      <c r="G8" s="430"/>
-      <c r="H8" s="430"/>
-      <c r="I8" s="428"/>
-      <c r="J8" s="428"/>
-      <c r="K8" s="429"/>
+      <c r="G8" s="448"/>
+      <c r="H8" s="448"/>
+      <c r="I8" s="446"/>
+      <c r="J8" s="446"/>
+      <c r="K8" s="447"/>
       <c r="L8" s="172" t="s">
         <v>338</v>
       </c>
@@ -6003,11 +6003,11 @@
       <c r="E9" s="136" t="s">
         <v>332</v>
       </c>
-      <c r="F9" s="449" t="s">
+      <c r="F9" s="409" t="s">
         <v>333</v>
       </c>
-      <c r="G9" s="450"/>
-      <c r="H9" s="451"/>
+      <c r="G9" s="410"/>
+      <c r="H9" s="411"/>
       <c r="I9" s="126" t="s">
         <v>335</v>
       </c>
@@ -6634,20 +6634,20 @@
       <c r="AC21" s="301"/>
     </row>
     <row r="22" spans="1:29" s="85" customFormat="1" ht="19" thickBot="1">
-      <c r="A22" s="417" t="s">
+      <c r="A22" s="435" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="418"/>
-      <c r="C22" s="417"/>
-      <c r="D22" s="419"/>
-      <c r="E22" s="420"/>
-      <c r="F22" s="417"/>
-      <c r="G22" s="419"/>
-      <c r="H22" s="419"/>
-      <c r="I22" s="419"/>
-      <c r="J22" s="419"/>
-      <c r="K22" s="420"/>
-      <c r="L22" s="417"/>
+      <c r="B22" s="436"/>
+      <c r="C22" s="435"/>
+      <c r="D22" s="437"/>
+      <c r="E22" s="438"/>
+      <c r="F22" s="435"/>
+      <c r="G22" s="437"/>
+      <c r="H22" s="437"/>
+      <c r="I22" s="437"/>
+      <c r="J22" s="437"/>
+      <c r="K22" s="438"/>
+      <c r="L22" s="435"/>
       <c r="M22" s="302"/>
       <c r="N22" s="81"/>
       <c r="O22" s="81"/>
@@ -6669,19 +6669,19 @@
       <c r="B23" s="212" t="s">
         <v>336</v>
       </c>
-      <c r="C23" s="431" t="s">
+      <c r="C23" s="449" t="s">
         <v>337</v>
       </c>
-      <c r="D23" s="432"/>
-      <c r="E23" s="433"/>
-      <c r="F23" s="431" t="s">
+      <c r="D23" s="450"/>
+      <c r="E23" s="451"/>
+      <c r="F23" s="449" t="s">
         <v>340</v>
       </c>
-      <c r="G23" s="434"/>
-      <c r="H23" s="434"/>
-      <c r="I23" s="432"/>
-      <c r="J23" s="432"/>
-      <c r="K23" s="433"/>
+      <c r="G23" s="452"/>
+      <c r="H23" s="452"/>
+      <c r="I23" s="450"/>
+      <c r="J23" s="450"/>
+      <c r="K23" s="451"/>
       <c r="L23" s="218" t="s">
         <v>338</v>
       </c>
@@ -6717,11 +6717,11 @@
       <c r="E24" s="217" t="s">
         <v>332</v>
       </c>
-      <c r="F24" s="452" t="s">
+      <c r="F24" s="412" t="s">
         <v>333</v>
       </c>
-      <c r="G24" s="453"/>
-      <c r="H24" s="454"/>
+      <c r="G24" s="413"/>
+      <c r="H24" s="414"/>
       <c r="I24" s="219" t="s">
         <v>335</v>
       </c>
@@ -7209,20 +7209,20 @@
       <c r="AC33" s="301"/>
     </row>
     <row r="34" spans="1:29" s="85" customFormat="1" ht="19" thickBot="1">
-      <c r="A34" s="413" t="s">
+      <c r="A34" s="431" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="414"/>
-      <c r="C34" s="413"/>
-      <c r="D34" s="415"/>
-      <c r="E34" s="416"/>
-      <c r="F34" s="413"/>
-      <c r="G34" s="415"/>
-      <c r="H34" s="415"/>
-      <c r="I34" s="415"/>
-      <c r="J34" s="415"/>
-      <c r="K34" s="416"/>
-      <c r="L34" s="413"/>
+      <c r="B34" s="432"/>
+      <c r="C34" s="431"/>
+      <c r="D34" s="433"/>
+      <c r="E34" s="434"/>
+      <c r="F34" s="431"/>
+      <c r="G34" s="433"/>
+      <c r="H34" s="433"/>
+      <c r="I34" s="433"/>
+      <c r="J34" s="433"/>
+      <c r="K34" s="434"/>
+      <c r="L34" s="431"/>
       <c r="M34" s="304"/>
       <c r="N34" s="131"/>
       <c r="O34" s="131"/>
@@ -7244,19 +7244,19 @@
       <c r="B35" s="222" t="s">
         <v>336</v>
       </c>
-      <c r="C35" s="442" t="s">
+      <c r="C35" s="405" t="s">
         <v>337</v>
       </c>
-      <c r="D35" s="443"/>
-      <c r="E35" s="444"/>
-      <c r="F35" s="442" t="s">
+      <c r="D35" s="407"/>
+      <c r="E35" s="408"/>
+      <c r="F35" s="405" t="s">
         <v>340</v>
       </c>
-      <c r="G35" s="448"/>
-      <c r="H35" s="448"/>
-      <c r="I35" s="443"/>
-      <c r="J35" s="443"/>
-      <c r="K35" s="444"/>
+      <c r="G35" s="406"/>
+      <c r="H35" s="406"/>
+      <c r="I35" s="407"/>
+      <c r="J35" s="407"/>
+      <c r="K35" s="408"/>
       <c r="L35" s="228" t="s">
         <v>338</v>
       </c>
@@ -7292,11 +7292,11 @@
       <c r="E36" s="227" t="s">
         <v>332</v>
       </c>
-      <c r="F36" s="455" t="s">
+      <c r="F36" s="415" t="s">
         <v>333</v>
       </c>
-      <c r="G36" s="456"/>
-      <c r="H36" s="457"/>
+      <c r="G36" s="416"/>
+      <c r="H36" s="417"/>
       <c r="I36" s="229" t="s">
         <v>335</v>
       </c>
@@ -9730,19 +9730,19 @@
       <c r="B84" s="248" t="s">
         <v>336</v>
       </c>
-      <c r="C84" s="402" t="s">
+      <c r="C84" s="421" t="s">
         <v>337</v>
       </c>
-      <c r="D84" s="403"/>
-      <c r="E84" s="404"/>
-      <c r="F84" s="402" t="s">
+      <c r="D84" s="422"/>
+      <c r="E84" s="423"/>
+      <c r="F84" s="421" t="s">
         <v>340</v>
       </c>
-      <c r="G84" s="405"/>
-      <c r="H84" s="405"/>
-      <c r="I84" s="403"/>
-      <c r="J84" s="403"/>
-      <c r="K84" s="404"/>
+      <c r="G84" s="420"/>
+      <c r="H84" s="420"/>
+      <c r="I84" s="422"/>
+      <c r="J84" s="422"/>
+      <c r="K84" s="423"/>
       <c r="L84" s="285" t="s">
         <v>338</v>
       </c>
@@ -9778,11 +9778,11 @@
       <c r="E85" s="251" t="s">
         <v>332</v>
       </c>
-      <c r="F85" s="458" t="s">
+      <c r="F85" s="418" t="s">
         <v>333</v>
       </c>
-      <c r="G85" s="459"/>
-      <c r="H85" s="405"/>
+      <c r="G85" s="419"/>
+      <c r="H85" s="420"/>
       <c r="I85" s="252" t="s">
         <v>335</v>
       </c>
@@ -10680,19 +10680,19 @@
       <c r="B107" s="193" t="s">
         <v>336</v>
       </c>
-      <c r="C107" s="406" t="s">
+      <c r="C107" s="424" t="s">
         <v>337</v>
       </c>
-      <c r="D107" s="407"/>
-      <c r="E107" s="408"/>
-      <c r="F107" s="406" t="s">
+      <c r="D107" s="425"/>
+      <c r="E107" s="426"/>
+      <c r="F107" s="424" t="s">
         <v>340</v>
       </c>
-      <c r="G107" s="409"/>
-      <c r="H107" s="409"/>
-      <c r="I107" s="407"/>
-      <c r="J107" s="407"/>
-      <c r="K107" s="408"/>
+      <c r="G107" s="427"/>
+      <c r="H107" s="427"/>
+      <c r="I107" s="425"/>
+      <c r="J107" s="425"/>
+      <c r="K107" s="426"/>
       <c r="L107" s="199" t="s">
         <v>338</v>
       </c>
@@ -10728,11 +10728,11 @@
       <c r="E108" s="198" t="s">
         <v>332</v>
       </c>
-      <c r="F108" s="445" t="s">
+      <c r="F108" s="402" t="s">
         <v>471</v>
       </c>
-      <c r="G108" s="446"/>
-      <c r="H108" s="447"/>
+      <c r="G108" s="403"/>
+      <c r="H108" s="404"/>
       <c r="I108" s="200" t="s">
         <v>472</v>
       </c>
@@ -11203,12 +11203,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F85:H85"/>
     <mergeCell ref="C84:E84"/>
     <mergeCell ref="F84:K84"/>
     <mergeCell ref="C107:E107"/>
@@ -11225,6 +11219,12 @@
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F85:H85"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11241,9 +11241,9 @@
   <dimension ref="A1:Z163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="560" topLeftCell="A138" activePane="bottomLeft"/>
+      <pane ySplit="560" topLeftCell="A140" activePane="bottomLeft"/>
       <selection activeCell="V22" sqref="V22"/>
-      <selection pane="bottomLeft" activeCell="W28" sqref="W28:Z28"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11331,16 +11331,16 @@
         <f>"0x"&amp;DEC2HEX(A2,2)</f>
         <v>0x00</v>
       </c>
-      <c r="E2" s="473" t="s">
+      <c r="E2" s="471" t="s">
         <v>269</v>
       </c>
-      <c r="F2" s="473"/>
-      <c r="G2" s="473"/>
-      <c r="H2" s="473"/>
-      <c r="I2" s="473"/>
-      <c r="J2" s="473"/>
-      <c r="K2" s="473"/>
-      <c r="L2" s="473"/>
+      <c r="F2" s="471"/>
+      <c r="G2" s="471"/>
+      <c r="H2" s="471"/>
+      <c r="I2" s="471"/>
+      <c r="J2" s="471"/>
+      <c r="K2" s="471"/>
+      <c r="L2" s="471"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3">
@@ -11354,14 +11354,14 @@
         <f t="shared" ref="C3:C9" si="1">"0x"&amp;DEC2HEX(A3,2)</f>
         <v>0x01</v>
       </c>
-      <c r="E3" s="473"/>
-      <c r="F3" s="473"/>
-      <c r="G3" s="473"/>
-      <c r="H3" s="473"/>
-      <c r="I3" s="473"/>
-      <c r="J3" s="473"/>
-      <c r="K3" s="473"/>
-      <c r="L3" s="473"/>
+      <c r="E3" s="471"/>
+      <c r="F3" s="471"/>
+      <c r="G3" s="471"/>
+      <c r="H3" s="471"/>
+      <c r="I3" s="471"/>
+      <c r="J3" s="471"/>
+      <c r="K3" s="471"/>
+      <c r="L3" s="471"/>
     </row>
     <row r="4" spans="1:26">
       <c r="A4">
@@ -11375,14 +11375,14 @@
         <f t="shared" si="1"/>
         <v>0x02</v>
       </c>
-      <c r="E4" s="473"/>
-      <c r="F4" s="473"/>
-      <c r="G4" s="473"/>
-      <c r="H4" s="473"/>
-      <c r="I4" s="473"/>
-      <c r="J4" s="473"/>
-      <c r="K4" s="473"/>
-      <c r="L4" s="473"/>
+      <c r="E4" s="471"/>
+      <c r="F4" s="471"/>
+      <c r="G4" s="471"/>
+      <c r="H4" s="471"/>
+      <c r="I4" s="471"/>
+      <c r="J4" s="471"/>
+      <c r="K4" s="471"/>
+      <c r="L4" s="471"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5">
@@ -11396,14 +11396,14 @@
         <f t="shared" si="1"/>
         <v>0x03</v>
       </c>
-      <c r="E5" s="473"/>
-      <c r="F5" s="473"/>
-      <c r="G5" s="473"/>
-      <c r="H5" s="473"/>
-      <c r="I5" s="473"/>
-      <c r="J5" s="473"/>
-      <c r="K5" s="473"/>
-      <c r="L5" s="473"/>
+      <c r="E5" s="471"/>
+      <c r="F5" s="471"/>
+      <c r="G5" s="471"/>
+      <c r="H5" s="471"/>
+      <c r="I5" s="471"/>
+      <c r="J5" s="471"/>
+      <c r="K5" s="471"/>
+      <c r="L5" s="471"/>
     </row>
     <row r="6" spans="1:26">
       <c r="A6">
@@ -11417,14 +11417,14 @@
         <f t="shared" si="1"/>
         <v>0x04</v>
       </c>
-      <c r="E6" s="473"/>
-      <c r="F6" s="473"/>
-      <c r="G6" s="473"/>
-      <c r="H6" s="473"/>
-      <c r="I6" s="473"/>
-      <c r="J6" s="473"/>
-      <c r="K6" s="473"/>
-      <c r="L6" s="473"/>
+      <c r="E6" s="471"/>
+      <c r="F6" s="471"/>
+      <c r="G6" s="471"/>
+      <c r="H6" s="471"/>
+      <c r="I6" s="471"/>
+      <c r="J6" s="471"/>
+      <c r="K6" s="471"/>
+      <c r="L6" s="471"/>
     </row>
     <row r="7" spans="1:26">
       <c r="A7">
@@ -11438,14 +11438,14 @@
         <f t="shared" si="1"/>
         <v>0x05</v>
       </c>
-      <c r="E7" s="473"/>
-      <c r="F7" s="473"/>
-      <c r="G7" s="473"/>
-      <c r="H7" s="473"/>
-      <c r="I7" s="473"/>
-      <c r="J7" s="473"/>
-      <c r="K7" s="473"/>
-      <c r="L7" s="473"/>
+      <c r="E7" s="471"/>
+      <c r="F7" s="471"/>
+      <c r="G7" s="471"/>
+      <c r="H7" s="471"/>
+      <c r="I7" s="471"/>
+      <c r="J7" s="471"/>
+      <c r="K7" s="471"/>
+      <c r="L7" s="471"/>
     </row>
     <row r="8" spans="1:26">
       <c r="A8">
@@ -11459,14 +11459,14 @@
         <f t="shared" si="1"/>
         <v>0x06</v>
       </c>
-      <c r="E8" s="473"/>
-      <c r="F8" s="473"/>
-      <c r="G8" s="473"/>
-      <c r="H8" s="473"/>
-      <c r="I8" s="473"/>
-      <c r="J8" s="473"/>
-      <c r="K8" s="473"/>
-      <c r="L8" s="473"/>
+      <c r="E8" s="471"/>
+      <c r="F8" s="471"/>
+      <c r="G8" s="471"/>
+      <c r="H8" s="471"/>
+      <c r="I8" s="471"/>
+      <c r="J8" s="471"/>
+      <c r="K8" s="471"/>
+      <c r="L8" s="471"/>
     </row>
     <row r="9" spans="1:26">
       <c r="A9">
@@ -11480,14 +11480,14 @@
         <f t="shared" si="1"/>
         <v>0x07</v>
       </c>
-      <c r="E9" s="473"/>
-      <c r="F9" s="473"/>
-      <c r="G9" s="473"/>
-      <c r="H9" s="473"/>
-      <c r="I9" s="473"/>
-      <c r="J9" s="473"/>
-      <c r="K9" s="473"/>
-      <c r="L9" s="473"/>
+      <c r="E9" s="471"/>
+      <c r="F9" s="471"/>
+      <c r="G9" s="471"/>
+      <c r="H9" s="471"/>
+      <c r="I9" s="471"/>
+      <c r="J9" s="471"/>
+      <c r="K9" s="471"/>
+      <c r="L9" s="471"/>
     </row>
     <row r="10" spans="1:26">
       <c r="A10">
@@ -11501,14 +11501,14 @@
         <f t="shared" ref="C10:C11" si="2">"0x"&amp;DEC2HEX(A10,2)</f>
         <v>0x08</v>
       </c>
-      <c r="E10" s="473"/>
-      <c r="F10" s="473"/>
-      <c r="G10" s="473"/>
-      <c r="H10" s="473"/>
-      <c r="I10" s="473"/>
-      <c r="J10" s="473"/>
-      <c r="K10" s="473"/>
-      <c r="L10" s="473"/>
+      <c r="E10" s="471"/>
+      <c r="F10" s="471"/>
+      <c r="G10" s="471"/>
+      <c r="H10" s="471"/>
+      <c r="I10" s="471"/>
+      <c r="J10" s="471"/>
+      <c r="K10" s="471"/>
+      <c r="L10" s="471"/>
     </row>
     <row r="11" spans="1:26">
       <c r="A11">
@@ -11522,14 +11522,14 @@
         <f t="shared" si="2"/>
         <v>0x09</v>
       </c>
-      <c r="E11" s="474"/>
-      <c r="F11" s="474"/>
-      <c r="G11" s="474"/>
-      <c r="H11" s="474"/>
-      <c r="I11" s="474"/>
-      <c r="J11" s="474"/>
-      <c r="K11" s="474"/>
-      <c r="L11" s="474"/>
+      <c r="E11" s="472"/>
+      <c r="F11" s="472"/>
+      <c r="G11" s="472"/>
+      <c r="H11" s="472"/>
+      <c r="I11" s="472"/>
+      <c r="J11" s="472"/>
+      <c r="K11" s="472"/>
+      <c r="L11" s="472"/>
     </row>
     <row r="12" spans="1:26">
       <c r="A12">
@@ -11543,18 +11543,18 @@
         <f t="shared" ref="C12:C23" si="3">"0x"&amp;DEC2HEX(A12,2)</f>
         <v>0x20</v>
       </c>
-      <c r="E12" s="471" t="s">
+      <c r="E12" s="478" t="s">
         <v>207</v>
       </c>
-      <c r="F12" s="471"/>
-      <c r="G12" s="471"/>
-      <c r="H12" s="471"/>
-      <c r="I12" s="471" t="s">
+      <c r="F12" s="478"/>
+      <c r="G12" s="478"/>
+      <c r="H12" s="478"/>
+      <c r="I12" s="478" t="s">
         <v>208</v>
       </c>
-      <c r="J12" s="471"/>
-      <c r="K12" s="471"/>
-      <c r="L12" s="471"/>
+      <c r="J12" s="478"/>
+      <c r="K12" s="478"/>
+      <c r="L12" s="478"/>
     </row>
     <row r="13" spans="1:26">
       <c r="A13">
@@ -11598,11 +11598,11 @@
       <c r="I14" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="J14" s="471" t="s">
+      <c r="J14" s="478" t="s">
         <v>209</v>
       </c>
-      <c r="K14" s="471"/>
-      <c r="L14" s="471"/>
+      <c r="K14" s="478"/>
+      <c r="L14" s="478"/>
     </row>
     <row r="15" spans="1:26">
       <c r="A15">
@@ -11616,16 +11616,16 @@
         <f t="shared" si="3"/>
         <v>0x24</v>
       </c>
-      <c r="E15" s="471" t="s">
+      <c r="E15" s="478" t="s">
         <v>210</v>
       </c>
-      <c r="F15" s="471"/>
-      <c r="G15" s="471"/>
-      <c r="H15" s="471"/>
-      <c r="I15" s="471"/>
-      <c r="J15" s="471"/>
-      <c r="K15" s="471"/>
-      <c r="L15" s="471"/>
+      <c r="F15" s="478"/>
+      <c r="G15" s="478"/>
+      <c r="H15" s="478"/>
+      <c r="I15" s="478"/>
+      <c r="J15" s="478"/>
+      <c r="K15" s="478"/>
+      <c r="L15" s="478"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16">
@@ -11639,16 +11639,16 @@
         <f t="shared" si="3"/>
         <v>0x25</v>
       </c>
-      <c r="E16" s="472"/>
-      <c r="F16" s="472"/>
-      <c r="G16" s="472"/>
-      <c r="H16" s="472"/>
-      <c r="I16" s="472"/>
-      <c r="J16" s="472"/>
-      <c r="K16" s="471" t="s">
+      <c r="E16" s="479"/>
+      <c r="F16" s="479"/>
+      <c r="G16" s="479"/>
+      <c r="H16" s="479"/>
+      <c r="I16" s="479"/>
+      <c r="J16" s="479"/>
+      <c r="K16" s="478" t="s">
         <v>211</v>
       </c>
-      <c r="L16" s="471"/>
+      <c r="L16" s="478"/>
     </row>
     <row r="17" spans="1:26">
       <c r="A17">
@@ -11662,16 +11662,16 @@
         <f t="shared" si="3"/>
         <v>0x26</v>
       </c>
-      <c r="E17" s="471" t="s">
+      <c r="E17" s="478" t="s">
         <v>212</v>
       </c>
-      <c r="F17" s="471"/>
-      <c r="G17" s="471"/>
-      <c r="H17" s="471"/>
-      <c r="I17" s="471"/>
-      <c r="J17" s="471"/>
-      <c r="K17" s="471"/>
-      <c r="L17" s="471"/>
+      <c r="F17" s="478"/>
+      <c r="G17" s="478"/>
+      <c r="H17" s="478"/>
+      <c r="I17" s="478"/>
+      <c r="J17" s="478"/>
+      <c r="K17" s="478"/>
+      <c r="L17" s="478"/>
     </row>
     <row r="18" spans="1:26">
       <c r="A18">
@@ -11812,18 +11812,18 @@
         <f t="shared" si="3"/>
         <v>0x2C</v>
       </c>
-      <c r="E23" s="471" t="s">
+      <c r="E23" s="478" t="s">
         <v>225</v>
       </c>
-      <c r="F23" s="471"/>
-      <c r="G23" s="471"/>
-      <c r="H23" s="471"/>
-      <c r="I23" s="471" t="s">
+      <c r="F23" s="478"/>
+      <c r="G23" s="478"/>
+      <c r="H23" s="478"/>
+      <c r="I23" s="478" t="s">
         <v>226</v>
       </c>
-      <c r="J23" s="471"/>
-      <c r="K23" s="471"/>
-      <c r="L23" s="471"/>
+      <c r="J23" s="478"/>
+      <c r="K23" s="478"/>
+      <c r="L23" s="478"/>
     </row>
     <row r="24" spans="1:26">
       <c r="A24">
@@ -11837,16 +11837,16 @@
         <f t="shared" ref="C24:C25" si="5">"0x"&amp;DEC2HEX(A24,2)</f>
         <v>0x2D</v>
       </c>
-      <c r="E24" s="475" t="s">
+      <c r="E24" s="473" t="s">
         <v>267</v>
       </c>
-      <c r="F24" s="476"/>
-      <c r="G24" s="476"/>
-      <c r="H24" s="476"/>
-      <c r="I24" s="476"/>
-      <c r="J24" s="476"/>
-      <c r="K24" s="476"/>
-      <c r="L24" s="477"/>
+      <c r="F24" s="474"/>
+      <c r="G24" s="474"/>
+      <c r="H24" s="474"/>
+      <c r="I24" s="474"/>
+      <c r="J24" s="474"/>
+      <c r="K24" s="474"/>
+      <c r="L24" s="475"/>
     </row>
     <row r="25" spans="1:26">
       <c r="A25">
@@ -11860,14 +11860,14 @@
         <f t="shared" si="5"/>
         <v>0x2F</v>
       </c>
-      <c r="E25" s="478"/>
-      <c r="F25" s="474"/>
-      <c r="G25" s="474"/>
-      <c r="H25" s="474"/>
-      <c r="I25" s="474"/>
-      <c r="J25" s="474"/>
-      <c r="K25" s="474"/>
-      <c r="L25" s="479"/>
+      <c r="E25" s="476"/>
+      <c r="F25" s="472"/>
+      <c r="G25" s="472"/>
+      <c r="H25" s="472"/>
+      <c r="I25" s="472"/>
+      <c r="J25" s="472"/>
+      <c r="K25" s="472"/>
+      <c r="L25" s="477"/>
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="117"/>
@@ -18728,6 +18728,323 @@
     </row>
   </sheetData>
   <mergeCells count="341">
+    <mergeCell ref="G158:I158"/>
+    <mergeCell ref="J158:L158"/>
+    <mergeCell ref="J162:L162"/>
+    <mergeCell ref="G162:H162"/>
+    <mergeCell ref="G160:H160"/>
+    <mergeCell ref="J160:L160"/>
+    <mergeCell ref="G161:H161"/>
+    <mergeCell ref="J161:L161"/>
+    <mergeCell ref="U158:W158"/>
+    <mergeCell ref="U144:W144"/>
+    <mergeCell ref="X144:Z144"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="G156:I156"/>
+    <mergeCell ref="J156:L156"/>
+    <mergeCell ref="G157:I157"/>
+    <mergeCell ref="J157:L157"/>
+    <mergeCell ref="U145:W145"/>
+    <mergeCell ref="X145:Z145"/>
+    <mergeCell ref="U146:W146"/>
+    <mergeCell ref="X146:Z146"/>
+    <mergeCell ref="S148:Z148"/>
+    <mergeCell ref="S149:Z149"/>
+    <mergeCell ref="S150:Z150"/>
+    <mergeCell ref="U152:W152"/>
+    <mergeCell ref="X152:Z152"/>
+    <mergeCell ref="U153:W153"/>
+    <mergeCell ref="X153:Z153"/>
+    <mergeCell ref="U154:W154"/>
+    <mergeCell ref="X154:Z154"/>
+    <mergeCell ref="U156:W156"/>
+    <mergeCell ref="X156:Z156"/>
+    <mergeCell ref="U157:W157"/>
+    <mergeCell ref="X157:Z157"/>
+    <mergeCell ref="S136:V136"/>
+    <mergeCell ref="W136:Z136"/>
+    <mergeCell ref="S137:V137"/>
+    <mergeCell ref="W137:Z137"/>
+    <mergeCell ref="S138:V138"/>
+    <mergeCell ref="W138:Z138"/>
+    <mergeCell ref="S140:Z140"/>
+    <mergeCell ref="S141:Z141"/>
+    <mergeCell ref="S142:Z142"/>
+    <mergeCell ref="S129:V129"/>
+    <mergeCell ref="W129:Z129"/>
+    <mergeCell ref="S130:V130"/>
+    <mergeCell ref="W130:Z130"/>
+    <mergeCell ref="S132:V132"/>
+    <mergeCell ref="W132:Z132"/>
+    <mergeCell ref="S133:V133"/>
+    <mergeCell ref="W133:Z133"/>
+    <mergeCell ref="S134:V134"/>
+    <mergeCell ref="W134:Z134"/>
+    <mergeCell ref="S122:V122"/>
+    <mergeCell ref="W122:Z122"/>
+    <mergeCell ref="S124:V124"/>
+    <mergeCell ref="W124:Z124"/>
+    <mergeCell ref="S125:V125"/>
+    <mergeCell ref="W125:Z125"/>
+    <mergeCell ref="S126:V126"/>
+    <mergeCell ref="W126:Z126"/>
+    <mergeCell ref="S128:V128"/>
+    <mergeCell ref="W128:Z128"/>
+    <mergeCell ref="S116:V116"/>
+    <mergeCell ref="W116:Z116"/>
+    <mergeCell ref="S117:V117"/>
+    <mergeCell ref="W117:Z117"/>
+    <mergeCell ref="S118:V118"/>
+    <mergeCell ref="W118:Z118"/>
+    <mergeCell ref="S120:V120"/>
+    <mergeCell ref="W120:Z120"/>
+    <mergeCell ref="S121:V121"/>
+    <mergeCell ref="W121:Z121"/>
+    <mergeCell ref="S109:V109"/>
+    <mergeCell ref="W109:Z109"/>
+    <mergeCell ref="S110:V110"/>
+    <mergeCell ref="W110:Z110"/>
+    <mergeCell ref="S112:V112"/>
+    <mergeCell ref="W112:Z112"/>
+    <mergeCell ref="S113:V113"/>
+    <mergeCell ref="W113:Z113"/>
+    <mergeCell ref="S114:V114"/>
+    <mergeCell ref="W114:Z114"/>
+    <mergeCell ref="V97:Z97"/>
+    <mergeCell ref="V98:Z98"/>
+    <mergeCell ref="V100:Z100"/>
+    <mergeCell ref="V101:Z101"/>
+    <mergeCell ref="V102:Z102"/>
+    <mergeCell ref="V104:Z104"/>
+    <mergeCell ref="V105:Z105"/>
+    <mergeCell ref="V106:Z106"/>
+    <mergeCell ref="S108:V108"/>
+    <mergeCell ref="W108:Z108"/>
+    <mergeCell ref="V85:Z85"/>
+    <mergeCell ref="V86:Z86"/>
+    <mergeCell ref="V88:Z88"/>
+    <mergeCell ref="V89:Z89"/>
+    <mergeCell ref="V90:Z90"/>
+    <mergeCell ref="V92:Z92"/>
+    <mergeCell ref="V93:Z93"/>
+    <mergeCell ref="V94:Z94"/>
+    <mergeCell ref="V96:Z96"/>
+    <mergeCell ref="S74:T74"/>
+    <mergeCell ref="V74:Z74"/>
+    <mergeCell ref="V76:Z76"/>
+    <mergeCell ref="V77:Z77"/>
+    <mergeCell ref="V78:Z78"/>
+    <mergeCell ref="V80:Z80"/>
+    <mergeCell ref="V81:Z81"/>
+    <mergeCell ref="V82:Z82"/>
+    <mergeCell ref="V84:Z84"/>
+    <mergeCell ref="S68:T68"/>
+    <mergeCell ref="V68:Z68"/>
+    <mergeCell ref="S69:T69"/>
+    <mergeCell ref="V69:Z69"/>
+    <mergeCell ref="S70:T70"/>
+    <mergeCell ref="V70:Z70"/>
+    <mergeCell ref="S72:T72"/>
+    <mergeCell ref="V72:Z72"/>
+    <mergeCell ref="S73:T73"/>
+    <mergeCell ref="V73:Z73"/>
+    <mergeCell ref="S61:T61"/>
+    <mergeCell ref="V61:Z61"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="V62:Z62"/>
+    <mergeCell ref="S64:T64"/>
+    <mergeCell ref="V64:Z64"/>
+    <mergeCell ref="S65:T65"/>
+    <mergeCell ref="V65:Z65"/>
+    <mergeCell ref="S66:T66"/>
+    <mergeCell ref="V66:Z66"/>
+    <mergeCell ref="T50:Z50"/>
+    <mergeCell ref="T52:Z52"/>
+    <mergeCell ref="T53:Z53"/>
+    <mergeCell ref="T54:Z54"/>
+    <mergeCell ref="T56:Z56"/>
+    <mergeCell ref="T57:Z57"/>
+    <mergeCell ref="T58:Z58"/>
+    <mergeCell ref="S60:T60"/>
+    <mergeCell ref="V60:Z60"/>
+    <mergeCell ref="T41:V41"/>
+    <mergeCell ref="W41:Z41"/>
+    <mergeCell ref="T42:V42"/>
+    <mergeCell ref="W42:Z42"/>
+    <mergeCell ref="T44:Z44"/>
+    <mergeCell ref="T45:Z45"/>
+    <mergeCell ref="T46:Z46"/>
+    <mergeCell ref="T48:Z48"/>
+    <mergeCell ref="T49:Z49"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="T33:V33"/>
+    <mergeCell ref="W33:Z33"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="W34:Z34"/>
+    <mergeCell ref="F53:L53"/>
+    <mergeCell ref="F54:L54"/>
+    <mergeCell ref="F56:L56"/>
+    <mergeCell ref="F57:L57"/>
+    <mergeCell ref="F58:L58"/>
+    <mergeCell ref="E17:L17"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="F44:L44"/>
+    <mergeCell ref="F45:L45"/>
+    <mergeCell ref="F46:L46"/>
+    <mergeCell ref="F48:L48"/>
+    <mergeCell ref="F49:L49"/>
+    <mergeCell ref="F50:L50"/>
+    <mergeCell ref="F52:L52"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="H68:L68"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="I30:L30"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="I33:L33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="H61:L61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="H62:L62"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="H65:L65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="H66:L66"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="H60:L60"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="H74:L74"/>
+    <mergeCell ref="H76:L76"/>
+    <mergeCell ref="H77:L77"/>
+    <mergeCell ref="H78:L78"/>
+    <mergeCell ref="H80:L80"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="H69:L69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="H70:L70"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="H73:L73"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="H72:L72"/>
+    <mergeCell ref="H89:L89"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H81:L81"/>
+    <mergeCell ref="H82:L82"/>
+    <mergeCell ref="H84:L84"/>
+    <mergeCell ref="H85:L85"/>
+    <mergeCell ref="H86:L86"/>
+    <mergeCell ref="H88:L88"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="E108:H108"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="I120:L120"/>
+    <mergeCell ref="E113:H113"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="E114:H114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="E116:H116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="E109:H109"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="E110:H110"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="E112:H112"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="E128:H128"/>
+    <mergeCell ref="I128:L128"/>
+    <mergeCell ref="E129:H129"/>
+    <mergeCell ref="I129:L129"/>
+    <mergeCell ref="E130:H130"/>
+    <mergeCell ref="I130:L130"/>
+    <mergeCell ref="E2:L11"/>
+    <mergeCell ref="I124:L124"/>
+    <mergeCell ref="I125:L125"/>
+    <mergeCell ref="I126:L126"/>
+    <mergeCell ref="E124:H124"/>
+    <mergeCell ref="E125:H125"/>
+    <mergeCell ref="E126:H126"/>
+    <mergeCell ref="E121:H121"/>
+    <mergeCell ref="I121:L121"/>
+    <mergeCell ref="E122:H122"/>
+    <mergeCell ref="I122:L122"/>
+    <mergeCell ref="E24:L25"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="E117:H117"/>
+    <mergeCell ref="I117:L117"/>
+    <mergeCell ref="E118:H118"/>
+    <mergeCell ref="I118:L118"/>
+    <mergeCell ref="E120:H120"/>
+    <mergeCell ref="E136:H136"/>
+    <mergeCell ref="I136:L136"/>
+    <mergeCell ref="E137:H137"/>
+    <mergeCell ref="I137:L137"/>
+    <mergeCell ref="E138:H138"/>
+    <mergeCell ref="I138:L138"/>
+    <mergeCell ref="E132:H132"/>
+    <mergeCell ref="I132:L132"/>
+    <mergeCell ref="E133:H133"/>
+    <mergeCell ref="I133:L133"/>
+    <mergeCell ref="E134:H134"/>
+    <mergeCell ref="I134:L134"/>
+    <mergeCell ref="G146:I146"/>
+    <mergeCell ref="J146:L146"/>
+    <mergeCell ref="E140:L140"/>
+    <mergeCell ref="G144:I144"/>
+    <mergeCell ref="J144:L144"/>
+    <mergeCell ref="E141:L141"/>
+    <mergeCell ref="E142:L142"/>
+    <mergeCell ref="G145:I145"/>
+    <mergeCell ref="J145:L145"/>
+    <mergeCell ref="E148:L148"/>
+    <mergeCell ref="G152:I152"/>
+    <mergeCell ref="J152:L152"/>
+    <mergeCell ref="E149:L149"/>
+    <mergeCell ref="E150:L150"/>
+    <mergeCell ref="G153:I153"/>
+    <mergeCell ref="J153:L153"/>
+    <mergeCell ref="G154:I154"/>
+    <mergeCell ref="J154:L154"/>
     <mergeCell ref="X158:Z158"/>
     <mergeCell ref="U160:V160"/>
     <mergeCell ref="X160:Z160"/>
@@ -18752,323 +19069,6 @@
     <mergeCell ref="W38:Z38"/>
     <mergeCell ref="T40:V40"/>
     <mergeCell ref="W40:Z40"/>
-    <mergeCell ref="E148:L148"/>
-    <mergeCell ref="G152:I152"/>
-    <mergeCell ref="J152:L152"/>
-    <mergeCell ref="E149:L149"/>
-    <mergeCell ref="E150:L150"/>
-    <mergeCell ref="G153:I153"/>
-    <mergeCell ref="J153:L153"/>
-    <mergeCell ref="G154:I154"/>
-    <mergeCell ref="J154:L154"/>
-    <mergeCell ref="G146:I146"/>
-    <mergeCell ref="J146:L146"/>
-    <mergeCell ref="E140:L140"/>
-    <mergeCell ref="G144:I144"/>
-    <mergeCell ref="J144:L144"/>
-    <mergeCell ref="E141:L141"/>
-    <mergeCell ref="E142:L142"/>
-    <mergeCell ref="G145:I145"/>
-    <mergeCell ref="J145:L145"/>
-    <mergeCell ref="E136:H136"/>
-    <mergeCell ref="I136:L136"/>
-    <mergeCell ref="E137:H137"/>
-    <mergeCell ref="I137:L137"/>
-    <mergeCell ref="E138:H138"/>
-    <mergeCell ref="I138:L138"/>
-    <mergeCell ref="E132:H132"/>
-    <mergeCell ref="I132:L132"/>
-    <mergeCell ref="E133:H133"/>
-    <mergeCell ref="I133:L133"/>
-    <mergeCell ref="E134:H134"/>
-    <mergeCell ref="I134:L134"/>
-    <mergeCell ref="E128:H128"/>
-    <mergeCell ref="I128:L128"/>
-    <mergeCell ref="E129:H129"/>
-    <mergeCell ref="I129:L129"/>
-    <mergeCell ref="E130:H130"/>
-    <mergeCell ref="I130:L130"/>
-    <mergeCell ref="E2:L11"/>
-    <mergeCell ref="I124:L124"/>
-    <mergeCell ref="I125:L125"/>
-    <mergeCell ref="I126:L126"/>
-    <mergeCell ref="E124:H124"/>
-    <mergeCell ref="E125:H125"/>
-    <mergeCell ref="E126:H126"/>
-    <mergeCell ref="E121:H121"/>
-    <mergeCell ref="I121:L121"/>
-    <mergeCell ref="E122:H122"/>
-    <mergeCell ref="I122:L122"/>
-    <mergeCell ref="E24:L25"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E117:H117"/>
-    <mergeCell ref="I117:L117"/>
-    <mergeCell ref="E118:H118"/>
-    <mergeCell ref="I118:L118"/>
-    <mergeCell ref="E120:H120"/>
-    <mergeCell ref="I120:L120"/>
-    <mergeCell ref="E113:H113"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="E114:H114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="E116:H116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="E109:H109"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="E110:H110"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="E112:H112"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="H104:L104"/>
-    <mergeCell ref="H105:L105"/>
-    <mergeCell ref="H106:L106"/>
-    <mergeCell ref="E108:H108"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="H97:L97"/>
-    <mergeCell ref="H98:L98"/>
-    <mergeCell ref="H100:L100"/>
-    <mergeCell ref="H101:L101"/>
-    <mergeCell ref="H89:L89"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H81:L81"/>
-    <mergeCell ref="H82:L82"/>
-    <mergeCell ref="H84:L84"/>
-    <mergeCell ref="H85:L85"/>
-    <mergeCell ref="H86:L86"/>
-    <mergeCell ref="H88:L88"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="H74:L74"/>
-    <mergeCell ref="H76:L76"/>
-    <mergeCell ref="H77:L77"/>
-    <mergeCell ref="H78:L78"/>
-    <mergeCell ref="H80:L80"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="H69:L69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="H70:L70"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="H73:L73"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="H72:L72"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="H61:L61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="H62:L62"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="H65:L65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="H66:L66"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="H60:L60"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="H64:L64"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="H68:L68"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="I30:L30"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="I33:L33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:L34"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="F53:L53"/>
-    <mergeCell ref="F54:L54"/>
-    <mergeCell ref="F56:L56"/>
-    <mergeCell ref="F57:L57"/>
-    <mergeCell ref="F58:L58"/>
-    <mergeCell ref="E17:L17"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="F44:L44"/>
-    <mergeCell ref="F45:L45"/>
-    <mergeCell ref="F46:L46"/>
-    <mergeCell ref="F48:L48"/>
-    <mergeCell ref="F49:L49"/>
-    <mergeCell ref="F50:L50"/>
-    <mergeCell ref="F52:L52"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="E15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="T33:V33"/>
-    <mergeCell ref="W33:Z33"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="W34:Z34"/>
-    <mergeCell ref="T41:V41"/>
-    <mergeCell ref="W41:Z41"/>
-    <mergeCell ref="T42:V42"/>
-    <mergeCell ref="W42:Z42"/>
-    <mergeCell ref="T44:Z44"/>
-    <mergeCell ref="T45:Z45"/>
-    <mergeCell ref="T46:Z46"/>
-    <mergeCell ref="T48:Z48"/>
-    <mergeCell ref="T49:Z49"/>
-    <mergeCell ref="T50:Z50"/>
-    <mergeCell ref="T52:Z52"/>
-    <mergeCell ref="T53:Z53"/>
-    <mergeCell ref="T54:Z54"/>
-    <mergeCell ref="T56:Z56"/>
-    <mergeCell ref="T57:Z57"/>
-    <mergeCell ref="T58:Z58"/>
-    <mergeCell ref="S60:T60"/>
-    <mergeCell ref="V60:Z60"/>
-    <mergeCell ref="S61:T61"/>
-    <mergeCell ref="V61:Z61"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="V62:Z62"/>
-    <mergeCell ref="S64:T64"/>
-    <mergeCell ref="V64:Z64"/>
-    <mergeCell ref="S65:T65"/>
-    <mergeCell ref="V65:Z65"/>
-    <mergeCell ref="S66:T66"/>
-    <mergeCell ref="V66:Z66"/>
-    <mergeCell ref="S68:T68"/>
-    <mergeCell ref="V68:Z68"/>
-    <mergeCell ref="S69:T69"/>
-    <mergeCell ref="V69:Z69"/>
-    <mergeCell ref="S70:T70"/>
-    <mergeCell ref="V70:Z70"/>
-    <mergeCell ref="S72:T72"/>
-    <mergeCell ref="V72:Z72"/>
-    <mergeCell ref="S73:T73"/>
-    <mergeCell ref="V73:Z73"/>
-    <mergeCell ref="S74:T74"/>
-    <mergeCell ref="V74:Z74"/>
-    <mergeCell ref="V76:Z76"/>
-    <mergeCell ref="V77:Z77"/>
-    <mergeCell ref="V78:Z78"/>
-    <mergeCell ref="V80:Z80"/>
-    <mergeCell ref="V81:Z81"/>
-    <mergeCell ref="V82:Z82"/>
-    <mergeCell ref="V84:Z84"/>
-    <mergeCell ref="V85:Z85"/>
-    <mergeCell ref="V86:Z86"/>
-    <mergeCell ref="V88:Z88"/>
-    <mergeCell ref="V89:Z89"/>
-    <mergeCell ref="V90:Z90"/>
-    <mergeCell ref="V92:Z92"/>
-    <mergeCell ref="V93:Z93"/>
-    <mergeCell ref="V94:Z94"/>
-    <mergeCell ref="V96:Z96"/>
-    <mergeCell ref="V97:Z97"/>
-    <mergeCell ref="V98:Z98"/>
-    <mergeCell ref="V100:Z100"/>
-    <mergeCell ref="V101:Z101"/>
-    <mergeCell ref="V102:Z102"/>
-    <mergeCell ref="V104:Z104"/>
-    <mergeCell ref="V105:Z105"/>
-    <mergeCell ref="V106:Z106"/>
-    <mergeCell ref="S108:V108"/>
-    <mergeCell ref="W108:Z108"/>
-    <mergeCell ref="S109:V109"/>
-    <mergeCell ref="W109:Z109"/>
-    <mergeCell ref="S110:V110"/>
-    <mergeCell ref="W110:Z110"/>
-    <mergeCell ref="S112:V112"/>
-    <mergeCell ref="W112:Z112"/>
-    <mergeCell ref="S113:V113"/>
-    <mergeCell ref="W113:Z113"/>
-    <mergeCell ref="S114:V114"/>
-    <mergeCell ref="W114:Z114"/>
-    <mergeCell ref="S116:V116"/>
-    <mergeCell ref="W116:Z116"/>
-    <mergeCell ref="S117:V117"/>
-    <mergeCell ref="W117:Z117"/>
-    <mergeCell ref="S118:V118"/>
-    <mergeCell ref="W118:Z118"/>
-    <mergeCell ref="S120:V120"/>
-    <mergeCell ref="W120:Z120"/>
-    <mergeCell ref="S121:V121"/>
-    <mergeCell ref="W121:Z121"/>
-    <mergeCell ref="S122:V122"/>
-    <mergeCell ref="W122:Z122"/>
-    <mergeCell ref="S124:V124"/>
-    <mergeCell ref="W124:Z124"/>
-    <mergeCell ref="S125:V125"/>
-    <mergeCell ref="W125:Z125"/>
-    <mergeCell ref="S126:V126"/>
-    <mergeCell ref="W126:Z126"/>
-    <mergeCell ref="S128:V128"/>
-    <mergeCell ref="W128:Z128"/>
-    <mergeCell ref="S129:V129"/>
-    <mergeCell ref="W129:Z129"/>
-    <mergeCell ref="S130:V130"/>
-    <mergeCell ref="W130:Z130"/>
-    <mergeCell ref="S132:V132"/>
-    <mergeCell ref="W132:Z132"/>
-    <mergeCell ref="S133:V133"/>
-    <mergeCell ref="W133:Z133"/>
-    <mergeCell ref="S134:V134"/>
-    <mergeCell ref="W134:Z134"/>
-    <mergeCell ref="S136:V136"/>
-    <mergeCell ref="W136:Z136"/>
-    <mergeCell ref="S137:V137"/>
-    <mergeCell ref="W137:Z137"/>
-    <mergeCell ref="S138:V138"/>
-    <mergeCell ref="W138:Z138"/>
-    <mergeCell ref="S140:Z140"/>
-    <mergeCell ref="S141:Z141"/>
-    <mergeCell ref="S142:Z142"/>
-    <mergeCell ref="U144:W144"/>
-    <mergeCell ref="X144:Z144"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="G156:I156"/>
-    <mergeCell ref="J156:L156"/>
-    <mergeCell ref="G157:I157"/>
-    <mergeCell ref="J157:L157"/>
-    <mergeCell ref="U145:W145"/>
-    <mergeCell ref="X145:Z145"/>
-    <mergeCell ref="U146:W146"/>
-    <mergeCell ref="X146:Z146"/>
-    <mergeCell ref="S148:Z148"/>
-    <mergeCell ref="S149:Z149"/>
-    <mergeCell ref="S150:Z150"/>
-    <mergeCell ref="U152:W152"/>
-    <mergeCell ref="X152:Z152"/>
-    <mergeCell ref="U153:W153"/>
-    <mergeCell ref="X153:Z153"/>
-    <mergeCell ref="U154:W154"/>
-    <mergeCell ref="X154:Z154"/>
-    <mergeCell ref="U156:W156"/>
-    <mergeCell ref="X156:Z156"/>
-    <mergeCell ref="U157:W157"/>
-    <mergeCell ref="X157:Z157"/>
-    <mergeCell ref="G158:I158"/>
-    <mergeCell ref="J158:L158"/>
-    <mergeCell ref="J162:L162"/>
-    <mergeCell ref="G162:H162"/>
-    <mergeCell ref="G160:H160"/>
-    <mergeCell ref="J160:L160"/>
-    <mergeCell ref="G161:H161"/>
-    <mergeCell ref="J161:L161"/>
-    <mergeCell ref="U158:W158"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -19082,9 +19082,638 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="257" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="254" customFormat="1" ht="20">
+      <c r="A1" s="254" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="254" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" s="480" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="480"/>
+      <c r="E1" s="480"/>
+      <c r="F1" s="254" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="254" customFormat="1" ht="20">
+      <c r="C2" s="254" t="s">
+        <v>344</v>
+      </c>
+      <c r="D2" s="255" t="s">
+        <v>343</v>
+      </c>
+      <c r="E2" s="254" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="71" customFormat="1" ht="18">
+      <c r="D3" s="256"/>
+      <c r="F3" s="253" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="258" t="str">
+        <f>"B"&amp;DEC2BIN(C4,8)</f>
+        <v>B00000000</v>
+      </c>
+      <c r="E4" s="65" t="str">
+        <f>"0x"&amp;DEC2HEX(C4,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="258" t="str">
+        <f t="shared" ref="D5:D11" si="0">"B"&amp;DEC2BIN(C5,8)</f>
+        <v>B00000001</v>
+      </c>
+      <c r="E5" s="65" t="str">
+        <f t="shared" ref="E5:E11" si="1">"0x"&amp;DEC2HEX(C5,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000010</v>
+      </c>
+      <c r="E6" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x02</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000011</v>
+      </c>
+      <c r="E7" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x03</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000100</v>
+      </c>
+      <c r="E8" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x04</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000101</v>
+      </c>
+      <c r="E9" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x05</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000110</v>
+      </c>
+      <c r="E10" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x06</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" s="258" t="str">
+        <f t="shared" si="0"/>
+        <v>B00000111</v>
+      </c>
+      <c r="E11" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x07</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18">
+      <c r="F13" s="253" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="258" t="str">
+        <f>"B"&amp;DEC2BIN(C14,8)</f>
+        <v>B00000000</v>
+      </c>
+      <c r="E14" s="65" t="str">
+        <f>"0x"&amp;DEC2HEX(C14,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="258" t="str">
+        <f t="shared" ref="D15" si="2">"B"&amp;DEC2BIN(C15,8)</f>
+        <v>B00000001</v>
+      </c>
+      <c r="E15" s="65" t="str">
+        <f t="shared" ref="E15" si="3">"0x"&amp;DEC2HEX(C15,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="F15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="F16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" ht="18">
+      <c r="C18" s="65"/>
+      <c r="D18" s="258"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="260" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="258" t="str">
+        <f>"B"&amp;DEC2BIN(C19,8)</f>
+        <v>B00000000</v>
+      </c>
+      <c r="E19" s="65" t="str">
+        <f>"0x"&amp;DEC2HEX(C19,2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="F19" s="67" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="C20" s="65">
+        <v>1</v>
+      </c>
+      <c r="D20" s="258" t="str">
+        <f t="shared" ref="D20:D26" si="4">"B"&amp;DEC2BIN(C20,8)</f>
+        <v>B00000001</v>
+      </c>
+      <c r="E20" s="65" t="str">
+        <f t="shared" ref="E20:E26" si="5">"0x"&amp;DEC2HEX(C20,2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="F20" s="67" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
+      <c r="C21" s="65">
+        <v>2</v>
+      </c>
+      <c r="D21" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000010</v>
+      </c>
+      <c r="E21" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x02</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="65">
+        <v>3</v>
+      </c>
+      <c r="D22" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000011</v>
+      </c>
+      <c r="E22" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x03</v>
+      </c>
+      <c r="F22" s="67" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="65">
+        <v>4</v>
+      </c>
+      <c r="D23" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000100</v>
+      </c>
+      <c r="E23" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x04</v>
+      </c>
+      <c r="F23" s="67" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="C24" s="65">
+        <v>5</v>
+      </c>
+      <c r="D24" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000101</v>
+      </c>
+      <c r="E24" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x05</v>
+      </c>
+      <c r="F24" s="67" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="65">
+        <v>6</v>
+      </c>
+      <c r="D25" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000110</v>
+      </c>
+      <c r="E25" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x06</v>
+      </c>
+      <c r="F25" s="67" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="65">
+        <v>7</v>
+      </c>
+      <c r="D26" s="258" t="str">
+        <f t="shared" si="4"/>
+        <v>B00000111</v>
+      </c>
+      <c r="E26" s="65" t="str">
+        <f t="shared" si="5"/>
+        <v>0x07</v>
+      </c>
+      <c r="F26" s="67" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12">
+      <c r="G27" s="262"/>
+      <c r="H27" s="262"/>
+      <c r="I27" s="262"/>
+      <c r="J27" s="262"/>
+      <c r="K27" s="262"/>
+      <c r="L27" s="262"/>
+    </row>
+    <row r="28" spans="3:12" ht="18">
+      <c r="F28" s="261" t="s">
+        <v>353</v>
+      </c>
+      <c r="G28" s="263"/>
+      <c r="H28" s="263"/>
+      <c r="I28" s="263"/>
+      <c r="J28" s="263"/>
+      <c r="K28" s="263"/>
+      <c r="L28" s="263"/>
+    </row>
+    <row r="29" spans="3:12">
+      <c r="F29" s="259" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="F30" s="259" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="F31" s="259"/>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="F32" s="259"/>
+    </row>
+    <row r="34" spans="5:8">
+      <c r="E34" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="F34" s="67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8">
+      <c r="E35" s="65">
+        <v>0</v>
+      </c>
+      <c r="F35" s="67" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8">
+      <c r="E36" s="65">
+        <v>1</v>
+      </c>
+      <c r="F36" s="67" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8">
+      <c r="E37" s="65">
+        <v>2</v>
+      </c>
+      <c r="F37" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8">
+      <c r="E38" s="65">
+        <v>3</v>
+      </c>
+      <c r="F38" s="67" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8">
+      <c r="F39" s="481" t="s">
+        <v>279</v>
+      </c>
+      <c r="G39" s="481"/>
+      <c r="H39" s="70"/>
+    </row>
+    <row r="40" spans="5:8">
+      <c r="F40" s="482" t="s">
+        <v>280</v>
+      </c>
+      <c r="G40" s="482"/>
+      <c r="H40" s="482"/>
+    </row>
+    <row r="41" spans="5:8">
+      <c r="F41" s="481" t="s">
+        <v>261</v>
+      </c>
+      <c r="G41" s="481"/>
+      <c r="H41" s="481"/>
+    </row>
+    <row r="43" spans="5:8">
+      <c r="E43" t="s">
+        <v>317</v>
+      </c>
+      <c r="F43" s="66"/>
+    </row>
+    <row r="44" spans="5:8">
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="66" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" spans="5:8">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="69" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="46" spans="5:8">
+      <c r="E46" t="s">
+        <v>312</v>
+      </c>
+      <c r="F46" s="69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="47" spans="5:8">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="5:8">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="69">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6">
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" s="69">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6">
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" s="69">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6">
+      <c r="F51" s="66"/>
+    </row>
+    <row r="52" spans="5:6">
+      <c r="F52" s="69" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6">
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="69" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6">
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" s="69" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="56" spans="5:6">
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" s="69" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="57" spans="5:6">
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57" s="69" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6">
+      <c r="E58">
+        <v>5</v>
+      </c>
+      <c r="F58" s="69" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="5:6">
+      <c r="E59">
+        <v>6</v>
+      </c>
+      <c r="F59" s="69" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="5:6">
+      <c r="E60">
+        <v>7</v>
+      </c>
+      <c r="F60" s="69" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="63" spans="5:6">
+      <c r="F63" s="113"/>
+    </row>
+    <row r="64" spans="5:6">
+      <c r="F64" s="113" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6">
+      <c r="F65" s="113" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6">
+      <c r="F66" s="113"/>
+    </row>
+    <row r="67" spans="6:6">
+      <c r="F67" s="113"/>
+    </row>
+    <row r="68" spans="6:6">
+      <c r="F68" s="113" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6">
+      <c r="F69" s="113"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="580" topLeftCell="A104" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1:E1048576"/>
       <selection pane="bottomLeft" activeCell="K129" sqref="K129"/>
@@ -22451,7 +23080,7 @@
         <v>0337</v>
       </c>
       <c r="K79" s="12" t="str">
-        <f t="shared" ref="K79:K129" si="8">"0x"&amp;DEC2HEX(HEX2DEC(I79)+HEX2DEC(J79),4)</f>
+        <f t="shared" ref="K79:K109" si="8">"0x"&amp;DEC2HEX(HEX2DEC(I79)+HEX2DEC(J79),4)</f>
         <v>0x2B37</v>
       </c>
       <c r="L79" s="399">
@@ -24663,7 +25292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -24861,633 +25490,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="257" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="254" customFormat="1" ht="20">
-      <c r="A1" s="254" t="s">
-        <v>349</v>
-      </c>
-      <c r="B1" s="254" t="s">
-        <v>350</v>
-      </c>
-      <c r="C1" s="480" t="s">
-        <v>348</v>
-      </c>
-      <c r="D1" s="480"/>
-      <c r="E1" s="480"/>
-      <c r="F1" s="254" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="254" customFormat="1" ht="20">
-      <c r="C2" s="254" t="s">
-        <v>344</v>
-      </c>
-      <c r="D2" s="255" t="s">
-        <v>343</v>
-      </c>
-      <c r="E2" s="254" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="71" customFormat="1" ht="18">
-      <c r="D3" s="256"/>
-      <c r="F3" s="253" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="258" t="str">
-        <f>"B"&amp;DEC2BIN(C4,8)</f>
-        <v>B00000000</v>
-      </c>
-      <c r="E4" s="65" t="str">
-        <f>"0x"&amp;DEC2HEX(C4,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="258" t="str">
-        <f t="shared" ref="D5:D11" si="0">"B"&amp;DEC2BIN(C5,8)</f>
-        <v>B00000001</v>
-      </c>
-      <c r="E5" s="65" t="str">
-        <f t="shared" ref="E5:E11" si="1">"0x"&amp;DEC2HEX(C5,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000010</v>
-      </c>
-      <c r="E6" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x02</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000011</v>
-      </c>
-      <c r="E7" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x03</v>
-      </c>
-      <c r="F7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000100</v>
-      </c>
-      <c r="E8" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x04</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000101</v>
-      </c>
-      <c r="E9" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x05</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000110</v>
-      </c>
-      <c r="E10" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x06</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11" s="258" t="str">
-        <f t="shared" si="0"/>
-        <v>B00000111</v>
-      </c>
-      <c r="E11" s="65" t="str">
-        <f t="shared" si="1"/>
-        <v>0x07</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18">
-      <c r="F13" s="253" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="258" t="str">
-        <f>"B"&amp;DEC2BIN(C14,8)</f>
-        <v>B00000000</v>
-      </c>
-      <c r="E14" s="65" t="str">
-        <f>"0x"&amp;DEC2HEX(C14,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="F14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="258" t="str">
-        <f t="shared" ref="D15" si="2">"B"&amp;DEC2BIN(C15,8)</f>
-        <v>B00000001</v>
-      </c>
-      <c r="E15" s="65" t="str">
-        <f t="shared" ref="E15" si="3">"0x"&amp;DEC2HEX(C15,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="F15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="F16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" ht="18">
-      <c r="C18" s="65"/>
-      <c r="D18" s="258"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="260" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12">
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" s="258" t="str">
-        <f>"B"&amp;DEC2BIN(C19,8)</f>
-        <v>B00000000</v>
-      </c>
-      <c r="E19" s="65" t="str">
-        <f>"0x"&amp;DEC2HEX(C19,2)</f>
-        <v>0x00</v>
-      </c>
-      <c r="F19" s="67" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12">
-      <c r="C20" s="65">
-        <v>1</v>
-      </c>
-      <c r="D20" s="258" t="str">
-        <f t="shared" ref="D20:D26" si="4">"B"&amp;DEC2BIN(C20,8)</f>
-        <v>B00000001</v>
-      </c>
-      <c r="E20" s="65" t="str">
-        <f t="shared" ref="E20:E26" si="5">"0x"&amp;DEC2HEX(C20,2)</f>
-        <v>0x01</v>
-      </c>
-      <c r="F20" s="67" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12">
-      <c r="C21" s="65">
-        <v>2</v>
-      </c>
-      <c r="D21" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000010</v>
-      </c>
-      <c r="E21" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x02</v>
-      </c>
-      <c r="F21" s="67" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="65">
-        <v>3</v>
-      </c>
-      <c r="D22" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000011</v>
-      </c>
-      <c r="E22" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x03</v>
-      </c>
-      <c r="F22" s="67" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12">
-      <c r="C23" s="65">
-        <v>4</v>
-      </c>
-      <c r="D23" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000100</v>
-      </c>
-      <c r="E23" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x04</v>
-      </c>
-      <c r="F23" s="67" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12">
-      <c r="C24" s="65">
-        <v>5</v>
-      </c>
-      <c r="D24" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000101</v>
-      </c>
-      <c r="E24" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x05</v>
-      </c>
-      <c r="F24" s="67" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="65">
-        <v>6</v>
-      </c>
-      <c r="D25" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000110</v>
-      </c>
-      <c r="E25" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x06</v>
-      </c>
-      <c r="F25" s="67" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12">
-      <c r="C26" s="65">
-        <v>7</v>
-      </c>
-      <c r="D26" s="258" t="str">
-        <f t="shared" si="4"/>
-        <v>B00000111</v>
-      </c>
-      <c r="E26" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v>0x07</v>
-      </c>
-      <c r="F26" s="67" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="27" spans="3:12">
-      <c r="G27" s="262"/>
-      <c r="H27" s="262"/>
-      <c r="I27" s="262"/>
-      <c r="J27" s="262"/>
-      <c r="K27" s="262"/>
-      <c r="L27" s="262"/>
-    </row>
-    <row r="28" spans="3:12" ht="18">
-      <c r="F28" s="261" t="s">
-        <v>353</v>
-      </c>
-      <c r="G28" s="263"/>
-      <c r="H28" s="263"/>
-      <c r="I28" s="263"/>
-      <c r="J28" s="263"/>
-      <c r="K28" s="263"/>
-      <c r="L28" s="263"/>
-    </row>
-    <row r="29" spans="3:12">
-      <c r="F29" s="259" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30" spans="3:12">
-      <c r="F30" s="259" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="3:12">
-      <c r="F31" s="259"/>
-    </row>
-    <row r="32" spans="3:12">
-      <c r="F32" s="259"/>
-    </row>
-    <row r="34" spans="5:8">
-      <c r="E34" s="65" t="s">
-        <v>255</v>
-      </c>
-      <c r="F34" s="67" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="5:8">
-      <c r="E35" s="65">
-        <v>0</v>
-      </c>
-      <c r="F35" s="67" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8">
-      <c r="E36" s="65">
-        <v>1</v>
-      </c>
-      <c r="F36" s="67" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8">
-      <c r="E37" s="65">
-        <v>2</v>
-      </c>
-      <c r="F37" s="67" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="38" spans="5:8">
-      <c r="E38" s="65">
-        <v>3</v>
-      </c>
-      <c r="F38" s="67" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="39" spans="5:8">
-      <c r="F39" s="481" t="s">
-        <v>279</v>
-      </c>
-      <c r="G39" s="481"/>
-      <c r="H39" s="70"/>
-    </row>
-    <row r="40" spans="5:8">
-      <c r="F40" s="482" t="s">
-        <v>280</v>
-      </c>
-      <c r="G40" s="482"/>
-      <c r="H40" s="482"/>
-    </row>
-    <row r="41" spans="5:8">
-      <c r="F41" s="481" t="s">
-        <v>261</v>
-      </c>
-      <c r="G41" s="481"/>
-      <c r="H41" s="481"/>
-    </row>
-    <row r="43" spans="5:8">
-      <c r="E43" t="s">
-        <v>317</v>
-      </c>
-      <c r="F43" s="66"/>
-    </row>
-    <row r="44" spans="5:8">
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="66" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="45" spans="5:8">
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" s="69" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="46" spans="5:8">
-      <c r="E46" t="s">
-        <v>312</v>
-      </c>
-      <c r="F46" s="69" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="47" spans="5:8">
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" s="69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="5:8">
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" s="69">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6">
-      <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="F49" s="69">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6">
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="F50" s="69">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6">
-      <c r="F51" s="66"/>
-    </row>
-    <row r="52" spans="5:6">
-      <c r="F52" s="69" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="53" spans="5:6">
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" s="69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="5:6">
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="69" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="55" spans="5:6">
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55" s="69" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="56" spans="5:6">
-      <c r="E56">
-        <v>3</v>
-      </c>
-      <c r="F56" s="69" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="57" spans="5:6">
-      <c r="E57">
-        <v>4</v>
-      </c>
-      <c r="F57" s="69" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="58" spans="5:6">
-      <c r="E58">
-        <v>5</v>
-      </c>
-      <c r="F58" s="69" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="59" spans="5:6">
-      <c r="E59">
-        <v>6</v>
-      </c>
-      <c r="F59" s="69" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="60" spans="5:6">
-      <c r="E60">
-        <v>7</v>
-      </c>
-      <c r="F60" s="69" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="63" spans="5:6">
-      <c r="F63" s="113"/>
-    </row>
-    <row r="64" spans="5:6">
-      <c r="F64" s="113" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="65" spans="6:6">
-      <c r="F65" s="113" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="66" spans="6:6">
-      <c r="F66" s="113"/>
-    </row>
-    <row r="67" spans="6:6">
-      <c r="F67" s="113"/>
-    </row>
-    <row r="68" spans="6:6">
-      <c r="F68" s="113" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="69" spans="6:6">
-      <c r="F69" s="113"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>